<commit_message>
Add CAAF Data backtest
</commit_message>
<xml_diff>
--- a/Configs.xlsx
+++ b/Configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanspeter.schrei\Code\hanspeter\bt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A37533-7D00-411B-87D9-D041E630FB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A8A42A-768E-4604-8B44-3CEF61346F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55170" yWindow="0" windowWidth="21630" windowHeight="21000" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
+    <workbookView xWindow="1080" yWindow="480" windowWidth="21600" windowHeight="12735" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Country</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F4CA1A-2639-4A90-83F8-307845B50683}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,13 +562,70 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D7">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add diversification measure plotting
</commit_message>
<xml_diff>
--- a/Configs.xlsx
+++ b/Configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanspeter.schrei\Code\hanspeter\bt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBC43A4-297D-40FD-9778-0DA063430A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFD3FAB-4C25-475F-9B43-77CC4704B103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19125" yWindow="1590" windowWidth="21630" windowHeight="12735" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
+    <workbookView xWindow="1080" yWindow="480" windowWidth="21600" windowHeight="12735" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>Country</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>No HY Credit Limit, same as 9</t>
+  </si>
+  <si>
+    <t>Add TE to MV</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F4CA1A-2639-4A90-83F8-307845B50683}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -832,6 +835,84 @@
       </c>
       <c r="G17" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>6.2740000000000004E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>6.2740000000000004E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>0.25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>6.2740000000000004E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>0.25</v>
+      </c>
+      <c r="I20" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed German to English
</commit_message>
<xml_diff>
--- a/Configs.xlsx
+++ b/Configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanspeter.schrei\Code\hanspeter\bt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFD3FAB-4C25-475F-9B43-77CC4704B103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D47A46B-B3A7-4779-8C5A-1997B70F4AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="480" windowWidth="21600" windowHeight="12735" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21240" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
   <si>
     <t>Country</t>
   </si>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F4CA1A-2639-4A90-83F8-307845B50683}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,6 +915,84 @@
         <v>17</v>
       </c>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.1</v>
+      </c>
+      <c r="E21">
+        <v>40</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D22">
+        <v>0.1</v>
+      </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+      <c r="E23">
+        <v>40</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>0.05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Commit prior to two-stage switch
</commit_message>
<xml_diff>
--- a/Configs.xlsx
+++ b/Configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanspeter.schrei\Code\hanspeter\bt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D47A46B-B3A7-4779-8C5A-1997B70F4AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67469284-5D20-4028-A1D8-A41D5DFE058F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21240" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
+    <workbookView xWindow="31200" yWindow="0" windowWidth="17100" windowHeight="17400" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="18">
   <si>
     <t>Country</t>
   </si>
@@ -441,15 +441,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F4CA1A-2639-4A90-83F8-307845B50683}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -993,6 +994,92 @@
         <v>0.05</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.1</v>
+      </c>
+      <c r="E24">
+        <v>40</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D25">
+        <v>0.1</v>
+      </c>
+      <c r="E25">
+        <v>40</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D26">
+        <v>0.1</v>
+      </c>
+      <c r="E26">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>6.2600000000000003E-2</v>
+      </c>
+      <c r="D27">
+        <v>0.1</v>
+      </c>
+      <c r="E27">
+        <v>40</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Add post trigger mechanism analytics
</commit_message>
<xml_diff>
--- a/Configs.xlsx
+++ b/Configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanspeter.schrei\Code\hanspeter\bt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67469284-5D20-4028-A1D8-A41D5DFE058F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0501370F-01EC-476F-AC15-85C4C91E4D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31200" yWindow="0" windowWidth="17100" windowHeight="17400" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
+    <workbookView xWindow="7170" yWindow="0" windowWidth="21630" windowHeight="17400" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="19">
   <si>
     <t>Country</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Add TE to MV</t>
+  </si>
+  <si>
+    <t>Add TE to MV, Triggering Mechanism</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F4CA1A-2639-4A90-83F8-307845B50683}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1008,7 @@
         <v>0.1</v>
       </c>
       <c r="E24">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
@@ -1078,6 +1081,199 @@
       </c>
       <c r="I27" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>0.08</v>
+      </c>
+      <c r="D28">
+        <v>0.01</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>0.08</v>
+      </c>
+      <c r="D29">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>0.08</v>
+      </c>
+      <c r="D30">
+        <v>0.01</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>0.08</v>
+      </c>
+      <c r="D31">
+        <v>0.1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>0.08</v>
+      </c>
+      <c r="D32">
+        <v>0.02</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>0.08</v>
+      </c>
+      <c r="D33">
+        <v>0.01</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>0.08</v>
+      </c>
+      <c r="D34">
+        <v>0.01</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>0.08</v>
+      </c>
+      <c r="D35">
+        <v>0.02</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prior to Epsilon Adjustment
</commit_message>
<xml_diff>
--- a/Configs.xlsx
+++ b/Configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanspeter.schrei\Code\hanspeter\bt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0501370F-01EC-476F-AC15-85C4C91E4D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69300246-7648-4F5B-8334-B6527B89C4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="0" windowWidth="21630" windowHeight="17400" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="21870" windowHeight="16995" xr2:uid="{A3E9384F-A44B-449C-8C26-F09C1C34BF03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="24">
   <si>
     <t>Country</t>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>Add TE to MV, Triggering Mechanism</t>
+  </si>
+  <si>
+    <t>Modified Alternatives data, -0.0035 adjustment</t>
+  </si>
+  <si>
+    <t>Additional Comment</t>
+  </si>
+  <si>
+    <t>Additional Backtest for CAAF 1.0 Base Configuration</t>
+  </si>
+  <si>
+    <t>Additional Backtest for CAAF 1.0 Base Configuration (without HY Constraint)</t>
+  </si>
+  <si>
+    <t>Target MD</t>
   </si>
 </sst>
 </file>
@@ -444,19 +459,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F4CA1A-2639-4A90-83F8-307845B50683}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -484,8 +500,11 @@
       <c r="I1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -508,7 +527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -531,7 +550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -554,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -577,7 +596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -600,7 +619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -623,7 +642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -646,7 +665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -669,7 +688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -689,7 +708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -712,7 +731,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -735,7 +754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -761,7 +780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -781,7 +800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -801,7 +820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1201,7 +1220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1227,7 +1246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1253,7 +1272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1274,6 +1293,574 @@
       </c>
       <c r="G35" t="s">
         <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>0.08</v>
+      </c>
+      <c r="D36">
+        <v>0.01</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I36" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>0.08</v>
+      </c>
+      <c r="D37">
+        <v>0.01</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>0.08</v>
+      </c>
+      <c r="D38">
+        <v>0.01</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>0.08</v>
+      </c>
+      <c r="D39">
+        <v>0.01</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>0.08</v>
+      </c>
+      <c r="D40">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>0.08</v>
+      </c>
+      <c r="D41">
+        <v>0.1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>0.08</v>
+      </c>
+      <c r="D42">
+        <v>0.02</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>0.08</v>
+      </c>
+      <c r="D43">
+        <v>0.1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <v>0.08</v>
+      </c>
+      <c r="D44">
+        <v>0.02</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>0.08</v>
+      </c>
+      <c r="D45">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>0.08</v>
+      </c>
+      <c r="D46">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>0.08</v>
+      </c>
+      <c r="D47">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>0.08</v>
+      </c>
+      <c r="D48">
+        <v>0.1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>0.08</v>
+      </c>
+      <c r="D49">
+        <v>0.02</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0.08</v>
+      </c>
+      <c r="D50">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>0.08</v>
+      </c>
+      <c r="D51">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <v>0.08</v>
+      </c>
+      <c r="D52">
+        <v>0.02</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>0.08</v>
+      </c>
+      <c r="D53">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I53" t="s">
+        <v>23</v>
+      </c>
+      <c r="J53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>0.08</v>
+      </c>
+      <c r="D54">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I54" t="s">
+        <v>23</v>
+      </c>
+      <c r="J54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <v>0.08</v>
+      </c>
+      <c r="D55">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" t="s">
+        <v>10</v>
+      </c>
+      <c r="H55">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>0.08</v>
+      </c>
+      <c r="D56">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>0.08</v>
+      </c>
+      <c r="D57">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <v>0.08</v>
+      </c>
+      <c r="D58">
+        <v>0.2</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" t="s">
+        <v>12</v>
+      </c>
+      <c r="I58" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>